<commit_message>
Added measurements from DAC readings
</commit_message>
<xml_diff>
--- a/doc/FPGA pinout/FPGA - BOARD pinout.xlsx
+++ b/doc/FPGA pinout/FPGA - BOARD pinout.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\risco\Documents\UPC\MET\NASA\dev\MATESSE_channel_card_repo\doc\FPGA pinout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\MATESSE_channel_card_repo\doc\FPGA pinout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4E8058-AA95-482B-9D98-3C29798DB96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9AD96C-3A60-4AF0-A29B-1347F42A657C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{D67D1309-CD53-4386-A5CE-AF76992C5B03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{D67D1309-CD53-4386-A5CE-AF76992C5B03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Measurements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="142">
   <si>
     <t>FPGA PIN</t>
   </si>
@@ -332,6 +333,135 @@
   </si>
   <si>
     <t>DAC SDI chip1, chip2, chip3</t>
+  </si>
+  <si>
+    <t>ADC Analog Input Channel 0</t>
+  </si>
+  <si>
+    <t>AIN0+</t>
+  </si>
+  <si>
+    <t>DAC U0</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>P$51</t>
+  </si>
+  <si>
+    <t>P$47</t>
+  </si>
+  <si>
+    <t>0000000000000000</t>
+  </si>
+  <si>
+    <t>0001000000000000</t>
+  </si>
+  <si>
+    <t>P$45</t>
+  </si>
+  <si>
+    <t>0010000000000000</t>
+  </si>
+  <si>
+    <t>Consumption</t>
+  </si>
+  <si>
+    <t>1111111111111111</t>
+  </si>
+  <si>
+    <t>DAC U1</t>
+  </si>
+  <si>
+    <t>DAC U20</t>
+  </si>
+  <si>
+    <t>DAC U21</t>
+  </si>
+  <si>
+    <t>DAC U22</t>
+  </si>
+  <si>
+    <t>DAC U23</t>
+  </si>
+  <si>
+    <t>P$43</t>
+  </si>
+  <si>
+    <t>P$41</t>
+  </si>
+  <si>
+    <t>P$39</t>
+  </si>
+  <si>
+    <t>P$37</t>
+  </si>
+  <si>
+    <t>P$32</t>
+  </si>
+  <si>
+    <t>P$30</t>
+  </si>
+  <si>
+    <t>P$28</t>
+  </si>
+  <si>
+    <t>P$26</t>
+  </si>
+  <si>
+    <t>P$24</t>
+  </si>
+  <si>
+    <t>P$22</t>
+  </si>
+  <si>
+    <t>P$20</t>
+  </si>
+  <si>
+    <t>P$18</t>
+  </si>
+  <si>
+    <t>P$16</t>
+  </si>
+  <si>
+    <t>P$14</t>
+  </si>
+  <si>
+    <t>P$12</t>
+  </si>
+  <si>
+    <t>P$10</t>
+  </si>
+  <si>
+    <t>P$8</t>
+  </si>
+  <si>
+    <t>P$6</t>
+  </si>
+  <si>
+    <t>P$4</t>
+  </si>
+  <si>
+    <t>P$2</t>
   </si>
 </sst>
 </file>
@@ -381,9 +511,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D63C23-55A7-4B31-B56D-65631814CD2B}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,322 +925,333 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
         <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
         <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1117,4 +1259,1463 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF98FD6-80C8-45E3-9185-4299A2F56CD4}">
+  <dimension ref="A1:I125"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="G118" sqref="G118"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>237503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7">
+        <v>4096</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8">
+        <v>4096</v>
+      </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>4096</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <v>4096</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F10">
+        <v>0.36299999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12">
+        <v>8192</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13">
+        <v>8192</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14">
+        <v>8192</v>
+      </c>
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15">
+        <v>8192</v>
+      </c>
+      <c r="D15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15">
+        <v>0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17">
+        <v>65535</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17">
+        <v>2.492</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18">
+        <v>65535</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19">
+        <v>65535</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19">
+        <v>2.4910000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20">
+        <v>65535</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20">
+        <v>2.581</v>
+      </c>
+      <c r="G20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28">
+        <v>4096</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29">
+        <v>4096</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30">
+        <v>4096</v>
+      </c>
+      <c r="D30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31">
+        <v>4096</v>
+      </c>
+      <c r="D31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33">
+        <v>8192</v>
+      </c>
+      <c r="D33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34">
+        <v>8192</v>
+      </c>
+      <c r="D34" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35">
+        <v>8192</v>
+      </c>
+      <c r="D35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36">
+        <v>8192</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38">
+        <v>65535</v>
+      </c>
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39">
+        <v>65535</v>
+      </c>
+      <c r="D39" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40">
+        <v>65535</v>
+      </c>
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41">
+        <v>65535</v>
+      </c>
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49">
+        <v>4096</v>
+      </c>
+      <c r="D49" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C50">
+        <v>4096</v>
+      </c>
+      <c r="D50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51">
+        <v>4096</v>
+      </c>
+      <c r="D51" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52">
+        <v>4096</v>
+      </c>
+      <c r="D52" t="s">
+        <v>107</v>
+      </c>
+      <c r="E52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54">
+        <v>8192</v>
+      </c>
+      <c r="D54" t="s">
+        <v>104</v>
+      </c>
+      <c r="E54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55">
+        <v>8192</v>
+      </c>
+      <c r="D55" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56">
+        <v>8192</v>
+      </c>
+      <c r="D56" t="s">
+        <v>106</v>
+      </c>
+      <c r="E56" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C57">
+        <v>8192</v>
+      </c>
+      <c r="D57" t="s">
+        <v>107</v>
+      </c>
+      <c r="E57" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59">
+        <v>65535</v>
+      </c>
+      <c r="D59" t="s">
+        <v>104</v>
+      </c>
+      <c r="E59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60">
+        <v>65535</v>
+      </c>
+      <c r="D60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61">
+        <v>65535</v>
+      </c>
+      <c r="D61" t="s">
+        <v>106</v>
+      </c>
+      <c r="E61" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62">
+        <v>65535</v>
+      </c>
+      <c r="D62" t="s">
+        <v>107</v>
+      </c>
+      <c r="E62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>106</v>
+      </c>
+      <c r="E67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" t="s">
+        <v>107</v>
+      </c>
+      <c r="E68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70">
+        <v>4096</v>
+      </c>
+      <c r="D70" t="s">
+        <v>104</v>
+      </c>
+      <c r="E70" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71">
+        <v>4096</v>
+      </c>
+      <c r="D71" t="s">
+        <v>105</v>
+      </c>
+      <c r="E71" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C72">
+        <v>4096</v>
+      </c>
+      <c r="D72" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C73">
+        <v>4096</v>
+      </c>
+      <c r="D73" t="s">
+        <v>107</v>
+      </c>
+      <c r="E73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C75">
+        <v>8192</v>
+      </c>
+      <c r="D75" t="s">
+        <v>104</v>
+      </c>
+      <c r="E75" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76">
+        <v>8192</v>
+      </c>
+      <c r="D76" t="s">
+        <v>105</v>
+      </c>
+      <c r="E76" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C77">
+        <v>8192</v>
+      </c>
+      <c r="D77" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C78">
+        <v>8192</v>
+      </c>
+      <c r="D78" t="s">
+        <v>107</v>
+      </c>
+      <c r="E78" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B80" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80">
+        <v>65535</v>
+      </c>
+      <c r="D80" t="s">
+        <v>104</v>
+      </c>
+      <c r="E80" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81">
+        <v>65535</v>
+      </c>
+      <c r="D81" t="s">
+        <v>105</v>
+      </c>
+      <c r="E81" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B82" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C82">
+        <v>65535</v>
+      </c>
+      <c r="D82" t="s">
+        <v>106</v>
+      </c>
+      <c r="E82" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B83" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C83">
+        <v>65535</v>
+      </c>
+      <c r="D83" t="s">
+        <v>107</v>
+      </c>
+      <c r="E83" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86" t="s">
+        <v>104</v>
+      </c>
+      <c r="E86" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" t="s">
+        <v>105</v>
+      </c>
+      <c r="E87" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88" t="s">
+        <v>106</v>
+      </c>
+      <c r="E88" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B91" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C91">
+        <v>4096</v>
+      </c>
+      <c r="D91" t="s">
+        <v>104</v>
+      </c>
+      <c r="E91" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C92">
+        <v>4096</v>
+      </c>
+      <c r="D92" t="s">
+        <v>105</v>
+      </c>
+      <c r="E92" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C93">
+        <v>4096</v>
+      </c>
+      <c r="D93" t="s">
+        <v>106</v>
+      </c>
+      <c r="E93" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C94">
+        <v>4096</v>
+      </c>
+      <c r="D94" t="s">
+        <v>107</v>
+      </c>
+      <c r="E94" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B96" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C96">
+        <v>8192</v>
+      </c>
+      <c r="D96" t="s">
+        <v>104</v>
+      </c>
+      <c r="E96" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B97" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C97">
+        <v>8192</v>
+      </c>
+      <c r="D97" t="s">
+        <v>105</v>
+      </c>
+      <c r="E97" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B98" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C98">
+        <v>8192</v>
+      </c>
+      <c r="D98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E98" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B99" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C99">
+        <v>8192</v>
+      </c>
+      <c r="D99" t="s">
+        <v>107</v>
+      </c>
+      <c r="E99" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B101" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C101">
+        <v>65535</v>
+      </c>
+      <c r="D101" t="s">
+        <v>104</v>
+      </c>
+      <c r="E101" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B102" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C102">
+        <v>65535</v>
+      </c>
+      <c r="D102" t="s">
+        <v>105</v>
+      </c>
+      <c r="E102" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B103" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C103">
+        <v>65535</v>
+      </c>
+      <c r="D103" t="s">
+        <v>106</v>
+      </c>
+      <c r="E103" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B104" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C104">
+        <v>65535</v>
+      </c>
+      <c r="D104" t="s">
+        <v>107</v>
+      </c>
+      <c r="E104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107" t="s">
+        <v>104</v>
+      </c>
+      <c r="E107" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B108" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108" t="s">
+        <v>105</v>
+      </c>
+      <c r="E108" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B109" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109" t="s">
+        <v>106</v>
+      </c>
+      <c r="E109" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B110" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E110" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B112" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C112">
+        <v>4096</v>
+      </c>
+      <c r="D112" t="s">
+        <v>104</v>
+      </c>
+      <c r="E112" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C113">
+        <v>4096</v>
+      </c>
+      <c r="D113" t="s">
+        <v>105</v>
+      </c>
+      <c r="E113" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B114" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114">
+        <v>4096</v>
+      </c>
+      <c r="D114" t="s">
+        <v>106</v>
+      </c>
+      <c r="E114" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B115" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C115">
+        <v>4096</v>
+      </c>
+      <c r="D115" t="s">
+        <v>107</v>
+      </c>
+      <c r="E115" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B117" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C117">
+        <v>8192</v>
+      </c>
+      <c r="D117" t="s">
+        <v>104</v>
+      </c>
+      <c r="E117" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B118" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C118">
+        <v>8192</v>
+      </c>
+      <c r="D118" t="s">
+        <v>105</v>
+      </c>
+      <c r="E118" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B119" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C119">
+        <v>8192</v>
+      </c>
+      <c r="D119" t="s">
+        <v>106</v>
+      </c>
+      <c r="E119" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B120" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C120">
+        <v>8192</v>
+      </c>
+      <c r="D120" t="s">
+        <v>107</v>
+      </c>
+      <c r="E120" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B122" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C122">
+        <v>65535</v>
+      </c>
+      <c r="D122" t="s">
+        <v>104</v>
+      </c>
+      <c r="E122" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B123" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C123">
+        <v>65535</v>
+      </c>
+      <c r="D123" t="s">
+        <v>105</v>
+      </c>
+      <c r="E123" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B124" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C124">
+        <v>65535</v>
+      </c>
+      <c r="D124" t="s">
+        <v>106</v>
+      </c>
+      <c r="E124" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B125" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C125">
+        <v>65535</v>
+      </c>
+      <c r="D125" t="s">
+        <v>107</v>
+      </c>
+      <c r="E125" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>